<commit_message>
Final commit - contains some framework and test level changes
</commit_message>
<xml_diff>
--- a/Browse/src/test/resources/dataProvider/TestData.xlsx
+++ b/Browse/src/test/resources/dataProvider/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\theScoreApp\Browse\src\test\resources\dataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{B5923012-B51D-47C2-867B-DA8A8AA00EBE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{23C8FB23-82DB-43B4-A2FE-8A4750F63A5E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="35844" windowHeight="20064" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -444,7 +444,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -469,11 +469,11 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -484,15 +484,11 @@
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="Welcome@123" xr:uid="{8A6F7726-9A15-4E37-A445-1BA22EB55445}"/>
-    <hyperlink ref="B2" r:id="rId2" display="gurjotahuja@gmail.com" xr:uid="{5DCD7B0D-0EFA-41E7-A8DF-DEC63195CEAC}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>